<commit_message>
moved excel data to dbsqlite3
</commit_message>
<xml_diff>
--- a/AIacademia/data_files/gpt4_recommender_gen_training_data.xlsx
+++ b/AIacademia/data_files/gpt4_recommender_gen_training_data.xlsx
@@ -413,10 +413,10 @@
         <v>Course General Info and About</v>
       </c>
       <c r="D1" t="str">
-        <v>general Course Prequisites</v>
+        <v>Prequisites</v>
       </c>
       <c r="E1" t="str">
-        <v>subject Course Prequisites</v>
+        <v/>
       </c>
     </row>
     <row r="2">
@@ -430,10 +430,10 @@
         <v>The Bachelor of Science in Agricultural Education &amp; Extension intertwines the principles of modern agriculture with the art of education and community outreach. Students delve into agricultural practices, sustainability, and innovative technologies, while also mastering skills to disseminate this knowledge to farmers, communities, and educational institutions. As the demand for sustainable farming and informed agricultural practices grows, graduates are poised to lead, educate, and empower communities towards better farming and sustainable futures.</v>
       </c>
       <c r="D2" t="str">
-        <v xml:space="preserve">applicants admission degree programme meet minimum general admission requirement either mean grade c+ kenya certificate secondary education ( kcse ) examination , 2 principal passes 1 subsidiary east african advanced certificate examination/ kenya advanced certificate education ( eace/ kace ) , equivalents </v>
+        <v>applicants admission degree programme meet minimum general admission requirement either mean grade c+ kenya certificate secondary education ( kcse ) examination , 2 principal passes 1 subsidiary east african advanced certificate examination/ kenya advanced certificate education ( eace/ kace ) , equivalents.  grade c plain must diploma relevant field . addition , candidate must least c+ biology/biological sciences c+ agriculture kcse examinations . 3. holder diploma credit agricultural education related field college university recognized maseno university .</v>
       </c>
       <c r="E2" t="str">
-        <v xml:space="preserve"> grade c plain must diploma relevant field . addition , candidate must least c+ biology/biological sciences c+ agriculture kcse examinations . 3. holder diploma credit agricultural education related field college university recognized maseno university .</v>
+        <v/>
       </c>
     </row>
     <row r="3">
@@ -464,10 +464,10 @@
         <v>The Bachelor of Arts in Counselling Psychology &amp; Information Technology is a unique blend of human psychology and the world of IT. The course equips students with foundational knowledge in psychological theories and counseling techniques, while also introducing them to the ever-evolving realm of information technology. As technology becomes increasingly integrated into mental health services, graduates are positioned to spearhead innovative solutions in e-counseling, teletherapy, and digital mental health platforms.</v>
       </c>
       <c r="D4" t="str">
-        <v xml:space="preserve">) </v>
+        <v xml:space="preserve"> ii ) applicants must minimum c+ kcse equivalent .iv ) applicants may admitted strength diploma social sciences , arts humanities recognized institution .</v>
       </c>
       <c r="E4" t="str">
-        <v xml:space="preserve"> applicants must satisfy minimum entry requirements admission university . ii ) applicants must minimum c+ kcse equivalent . ii ) applicants must satisfy entry requirements admission school arts social sciences , maseno university . iv ) applicants may admitted strength diploma social sciences , arts humanities recognized institution .</v>
+        <v/>
       </c>
     </row>
     <row r="5">
@@ -481,7 +481,7 @@
         <v>The Bachelor of Arts in Religion is an enlightening journey into the mosaic of beliefs, traditions, and practices that have shaped human civilizations for millennia. Through this comprehensive program, students explore the history, philosophy, and cultural contexts of various religious systems. From the ancient rituals of early societies to the modern theologies of today, the course paints a broad picture of the enduring role of spirituality in daily life. As the world becomes increasingly interconnected, there's a growing need for understanding and empathy, and this degree equips graduates with insights into the profound ways religion influences behavior, ethics, and social structures.</v>
       </c>
       <c r="D5" t="str">
-        <v xml:space="preserve">attain pass language kcse equivalent </v>
+        <v/>
       </c>
       <c r="E5" t="str">
         <v/>
@@ -549,10 +549,10 @@
         <v>bachelor business information technology ( bbit ) programme geared towards equipping graduates sufficient knowledge business management skills skills information technology . combines key aspects information technology ( covering areas software development , communications , networking , security , systems analysis , databases , etc . ) key facets business accounting , finance , economics , management , marketing , human resources , operations management . combination skills knowledge prepares graduates immediately productive modern it-based business environment . programme lays strong foundation candidates progressing graduate studies field .</v>
       </c>
       <c r="D9" t="str">
-        <v>aggregate grade c+ k</v>
+        <v>c.s.e . minimum grade c mathematics two principal passes “ ” level/kenya advanced certificates education ( kace ) cue/ nec recognized diploma holders related areas eligible join first year exemptions . equivalent qualifications approved school business economics university senate .</v>
       </c>
       <c r="E9" t="str">
-        <v>c.s.e . minimum grade c mathematics two principal passes “ ” level/kenya advanced certificates education ( kace ) cue/ nec recognized diploma holders related areas eligible join first year exemptions . equivalent qualifications approved school business economics university senate .</v>
+        <v/>
       </c>
     </row>
     <row r="10">
@@ -566,10 +566,10 @@
         <v>Every product has a journey, and understanding this journey is at the heart of the Bachelor of Supply Chain Management. This comprehensive program delves into the intricacies of procuring, producing, and delivering goods in today's globalized market. Students explore facets of logistics, inventory control, and distribution, gaining insights into the strategies that ensure smooth and efficient operations. As businesses strive for timely deliveries and streamlined processes, graduates of this program are primed to design and manage the sophisticated networks that make it all possible.</v>
       </c>
       <c r="D10" t="str">
-        <v xml:space="preserve">satisfy minimum entry requirements admission university </v>
+        <v xml:space="preserve"> obtained minimum grade c ( plain ) mathematics ksce equivalent .</v>
       </c>
       <c r="E10" t="str">
-        <v xml:space="preserve"> satisfy entry requirements admission school business economics maseno university additionally obtained minimum grade c ( plain ) mathematics ksce equivalent .</v>
+        <v/>
       </c>
     </row>
     <row r="11">
@@ -583,10 +583,10 @@
         <v>recent growth tourism kenya east african region requires competent dedicated human resources ability work various sectors hospitality related institutions region beyond . fast-changing nature hospitality tourism industry requires personnel capable understanding responsive ever-changing environment . background , course designed train produce graduates able meet industry demands .</v>
       </c>
       <c r="D11" t="str">
-        <v xml:space="preserve">university common admission requirements shall apply </v>
+        <v xml:space="preserve"> candidate shall scored least ) grade c+ ( c plus ) english/ kiswahili . addition , candidate must attained least c ( c plain ) mathematics kcse equivalents examinations . candidate scores minimum principal pass chemistry , biology , geography subsidiary passes either maths physics a-level examinations eligible . candidates credit pass ordinary diploma hospitality tourism management related courses recognized institution qualify .</v>
       </c>
       <c r="E11" t="str">
-        <v xml:space="preserve"> candidate shall scored least ) grade c+ ( c plus ) english/ kiswahili . addition , candidate must attained least c ( c plain ) mathematics kcse equivalents examinations . candidate scores minimum principal pass chemistry , biology , geography subsidiary passes either maths physics a-level examinations eligible . candidates credit pass ordinary diploma hospitality tourism management related courses recognized institution qualify .</v>
+        <v/>
       </c>
     </row>
     <row r="12">
@@ -600,10 +600,10 @@
         <v>recent growth tourism kenya called development human resources work various tourism hospitality firms country . programme provide skilled knowledgeable graduates employable operatives managers different tourism hospitality establishments kenya thus filling existing training needs gaps .</v>
       </c>
       <c r="D12" t="str">
-        <v xml:space="preserve">university common admission requirements shall apply </v>
+        <v xml:space="preserve"> candidate shall scored least ) grade c+ ( c plus ) english/ kiswahili . addition , candidate must attained least c ( c plain ) mathematics kcse equivalents examinations . candidate scores minimum principal pass chemistry , biology , geography subsidiary passes either maths physics a-level examinations eligible . candidates credit pass ordinary diploma hospitality tourism management related courses recognized institution qualify .</v>
       </c>
       <c r="E12" t="str">
-        <v xml:space="preserve"> candidate shall scored least ) grade c+ ( c plus ) english/ kiswahili . addition , candidate must attained least c ( c plain ) mathematics kcse equivalents examinations . candidate scores minimum principal pass chemistry , biology , geography subsidiary passes either maths physics a-level examinations eligible . candidates credit pass ordinary diploma hospitality tourism management related courses recognized institution qualify .</v>
+        <v/>
       </c>
     </row>
     <row r="13">
@@ -617,10 +617,10 @@
         <v>The Bachelor of Science in Computer Science is a voyage into the intricate realms of algorithms, programming, and digital systems. Throughout the program, students unravel the complexities of software development, diving deep into coding languages, data structures, and computational theories. They also engage with real-world projects, harnessing their analytical and creative skills to devise innovative solutions for complex problems. As the digital age continues to evolve, this degree stands as a beacon for those aiming to shape the future of technology, ensuring they possess both the foundational knowledge and the adaptive mindset required in this ever-changing field.</v>
       </c>
       <c r="D13" t="str">
-        <v xml:space="preserve">ksce mean grade c+ , least c+ mathematics physics/physical science , kace least 2 principles passes mathematics physics 1 subsidiary pass , accredited diploma computer science /it/ related field least credit pass commission higher education accredited validated institution </v>
+        <v>ksce mean grade c+ , least c+ mathematics physics/physical science , kace least 2 principles passes mathematics physics 1 subsidiary pass , accredited diploma computer science /it/ related field least credit pass commission higher education accredited validated institution.  knec diploma holders computer studies least credit pass mean grade c kcse .</v>
       </c>
       <c r="E13" t="str">
-        <v xml:space="preserve"> knec diploma holders computer studies least credit pass mean grade c kcse .</v>
+        <v/>
       </c>
     </row>
     <row r="14">
@@ -651,10 +651,10 @@
         <v>computer technology solidly grounded theories principles computing , mathematics , science , engineering . applies theories principles solve technical problems design computing hardware , firmware , networks , processes . department offers courses together university approved courses lead bachelor science degree computer technology . goal program produce computer technology graduates capable using computing theories , principles techniques design , implement , manage maintain computing systems provide various technical economic solutions benefit humankind . The Bachelor of Science in Computer Technology offers a focused look into the hardware and software that power today's technological innovations. With a blend of hands-on experience and theoretical insights, students are primed to bridge the gap between design and application in the tech world.</v>
       </c>
       <c r="D15" t="str">
-        <v xml:space="preserve">ksce mean grade c+ , least c+ mathematics physics/physical science , kace least 2 principles passes mathematics physics 1 subsidiary pass , accredited diploma computer science /it/ related field least credit pass commission higher education accredited validated institution </v>
+        <v>ksce mean grade c+ , least c+ mathematics physics/physical science , kace least 2 principles passes mathematics physics 1 subsidiary pass , accredited diploma computer science /it/ related field least credit pass commission higher education accredited validated institution.  knec diploma holders computer studies least credit pass mean grade c kcse .</v>
       </c>
       <c r="E15" t="str">
-        <v xml:space="preserve"> knec diploma holders computer studies least credit pass mean grade c kcse .</v>
+        <v/>
       </c>
     </row>
     <row r="16">
@@ -668,10 +668,10 @@
         <v>The Bachelor of Education in Early Childhood Development &amp; Education is a comprehensive exploration into the formative years of human development. This degree equips students with the insights and skills needed to foster the intellectual, emotional, and social growth of young children. Delving into pedagogical theories, developmental psychology, and hands-on teaching methodologies, graduates emerge prepared to shape the foundational experiences of young learners. In a world where early education plays a pivotal role in future success, this program stands as a beacon for those dedicated to nurturing the next generation from their earliest stages.</v>
       </c>
       <c r="D16" t="str">
-        <v>admitted programme , candidate must satisfy university entry requirements i</v>
+        <v>minimum mean grade c+ kcse two principal passes kace/eaace diploma certificate ecde knec diploma education recognized institution</v>
       </c>
       <c r="E16" t="str">
-        <v>e . minimum mean grade c+ kcse two principal passes kace/eaace diploma certificate ecde knec diploma education recognized institution</v>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>